<commit_message>
Publish site to docs/
</commit_message>
<xml_diff>
--- a/data/content.xlsx
+++ b/data/content.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Markus/Documents/GitHub/Inschriftenschluessel/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Markus/Documents/Arbeit/Inschriftenschluessel/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6316B353-F038-0541-B4EE-F8C27BAC3B2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DD6C280-7A04-7A44-8237-FC9735438255}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6760" yWindow="500" windowWidth="22040" windowHeight="16160" activeTab="4" xr2:uid="{F025A444-F8B0-5C41-A37E-BEE791B22240}"/>
+    <workbookView xWindow="-20" yWindow="500" windowWidth="28800" windowHeight="16100" activeTab="4" xr2:uid="{F025A444-F8B0-5C41-A37E-BEE791B22240}"/>
   </bookViews>
   <sheets>
     <sheet name="pages" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="512" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="510" uniqueCount="219">
   <si>
     <t>page_id</t>
   </si>
@@ -538,18 +538,9 @@
     <t>epitheta/01_m-jp.t/</t>
   </si>
   <si>
-    <t xml:space="preserve"> (Spät.)</t>
-  </si>
-  <si>
     <t>0001_m-jp.t_01</t>
   </si>
   <si>
-    <t>0010_m-jp.t_02</t>
-  </si>
-  <si>
-    <t>0020_m-jp.t_SP_01</t>
-  </si>
-  <si>
     <t>0001_Jmn-Ra_01</t>
   </si>
   <si>
@@ -689,6 +680,24 @@
   </si>
   <si>
     <t>Thot</t>
+  </si>
+  <si>
+    <t>collapsible-heading</t>
+  </si>
+  <si>
+    <t>Öffne Göttertabellen</t>
+  </si>
+  <si>
+    <t>[[table:tb_epith_001]]</t>
+  </si>
+  <si>
+    <t>tb_epith_001</t>
+  </si>
+  <si>
+    <t>*m jp.t*</t>
+  </si>
+  <si>
+    <t>(Amun) in Luxor</t>
   </si>
 </sst>
 </file>
@@ -1081,7 +1090,7 @@
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD14"/>
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="7.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1345,7 +1354,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1391,7 +1400,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1511,10 +1520,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AEDD5969-C8E3-C04D-AF17-FDEFB8218719}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="7.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1525,9 +1534,10 @@
     <col min="4" max="4" width="36.1640625" customWidth="1"/>
     <col min="5" max="5" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1546,8 +1556,11 @@
       <c r="F1" s="1" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G1" s="1" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -1561,7 +1574,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="85" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" ht="85" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -1575,7 +1588,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -1592,7 +1605,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -1607,6 +1620,9 @@
       </c>
       <c r="F5" t="s">
         <v>66</v>
+      </c>
+      <c r="G5" t="s">
+        <v>214</v>
       </c>
     </row>
   </sheetData>
@@ -1618,8 +1634,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C62D4F70-2351-5545-A291-11D662F747FD}">
   <dimension ref="A1:K84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="117" workbookViewId="0">
-      <selection activeCell="C43" sqref="C43:C84"/>
+    <sheetView tabSelected="1" topLeftCell="C12" zoomScale="117" workbookViewId="0">
+      <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1629,7 +1645,7 @@
     <col min="3" max="3" width="22.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="3.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="45" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.1640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="19.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="4.5" bestFit="1" customWidth="1"/>
     <col min="9" max="10" width="4.5" customWidth="1"/>
@@ -2130,48 +2146,8 @@
       <c r="C29" t="s">
         <v>145</v>
       </c>
-      <c r="E29" t="s">
-        <v>148</v>
-      </c>
-      <c r="F29" t="s">
-        <v>164</v>
-      </c>
-      <c r="G29" t="s">
-        <v>166</v>
-      </c>
-      <c r="H29" t="s">
-        <v>151</v>
-      </c>
-      <c r="K29" t="str">
-        <f>_xlfn.TEXTJOIN("", TRUE, D29:J29)</f>
-        <v>02_Slots/Gottheit/Goetter-mit-Epitheta/0001_Amun/epitheta/01_m-jp.t/0001_m-jp.t_01.png</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>65</v>
-      </c>
-      <c r="B30">
-        <v>1</v>
-      </c>
-      <c r="C30" t="s">
-        <v>145</v>
-      </c>
-      <c r="E30" t="s">
-        <v>148</v>
-      </c>
-      <c r="F30" t="s">
-        <v>164</v>
-      </c>
-      <c r="G30" t="s">
-        <v>167</v>
-      </c>
-      <c r="H30" t="s">
-        <v>151</v>
-      </c>
-      <c r="K30" t="str">
-        <f>_xlfn.TEXTJOIN("", TRUE, D30:J30)</f>
-        <v>02_Slots/Gottheit/Goetter-mit-Epitheta/0001_Amun/epitheta/01_m-jp.t/0010_m-jp.t_02.png</v>
+      <c r="K29" t="s">
+        <v>215</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.2">
@@ -2179,29 +2155,40 @@
         <v>65</v>
       </c>
       <c r="B31">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C31" t="s">
-        <v>145</v>
-      </c>
-      <c r="E31" t="s">
-        <v>148</v>
-      </c>
-      <c r="F31" t="s">
-        <v>164</v>
+        <v>43</v>
       </c>
       <c r="G31" t="s">
+        <v>166</v>
+      </c>
+      <c r="K31" t="s">
         <v>168</v>
       </c>
-      <c r="H31" t="s">
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>65</v>
+      </c>
+      <c r="B32">
+        <v>10</v>
+      </c>
+      <c r="C32" t="s">
+        <v>142</v>
+      </c>
+      <c r="E32" t="s">
+        <v>169</v>
+      </c>
+      <c r="G32" t="s">
+        <v>166</v>
+      </c>
+      <c r="H32" t="s">
         <v>151</v>
       </c>
-      <c r="J31" t="s">
-        <v>165</v>
-      </c>
-      <c r="K31" t="str">
-        <f>_xlfn.TEXTJOIN("", TRUE, D31:J31)</f>
-        <v>02_Slots/Gottheit/Goetter-mit-Epitheta/0001_Amun/epitheta/01_m-jp.t/0020_m-jp.t_SP_01.png (Spät.)</v>
+      <c r="K32" t="str">
+        <f>_xlfn.TEXTJOIN("", TRUE, D32:J32)</f>
+        <v>02_Slots/Gottheit/Goetter-mit-Epitheta/0010_Amun-Re/0001_Jmn-Ra_01.png</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.2">
@@ -2212,13 +2199,7 @@
         <v>10</v>
       </c>
       <c r="C33" t="s">
-        <v>43</v>
-      </c>
-      <c r="G33" t="s">
-        <v>169</v>
-      </c>
-      <c r="K33" t="s">
-        <v>171</v>
+        <v>143</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.2">
@@ -2229,20 +2210,10 @@
         <v>10</v>
       </c>
       <c r="C34" t="s">
-        <v>142</v>
-      </c>
-      <c r="E34" t="s">
-        <v>172</v>
-      </c>
-      <c r="G34" t="s">
-        <v>169</v>
-      </c>
-      <c r="H34" t="s">
-        <v>151</v>
-      </c>
-      <c r="K34" t="str">
-        <f>_xlfn.TEXTJOIN("", TRUE, D34:J34)</f>
-        <v>02_Slots/Gottheit/Goetter-mit-Epitheta/0010_Amun-Re/0001_Jmn-Ra_01.png</v>
+        <v>144</v>
+      </c>
+      <c r="K34" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.2">
@@ -2253,32 +2224,62 @@
         <v>10</v>
       </c>
       <c r="C35" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>65</v>
-      </c>
-      <c r="B36">
-        <v>10</v>
-      </c>
-      <c r="C36" t="s">
-        <v>144</v>
-      </c>
-      <c r="K36" t="s">
-        <v>170</v>
+        <v>145</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>65</v>
+        <v>216</v>
       </c>
       <c r="B37">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="C37" t="s">
-        <v>145</v>
+        <v>43</v>
+      </c>
+      <c r="K37" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>216</v>
+      </c>
+      <c r="B38">
+        <v>1</v>
+      </c>
+      <c r="C38" t="s">
+        <v>142</v>
+      </c>
+      <c r="E38" t="s">
+        <v>148</v>
+      </c>
+      <c r="F38" t="s">
+        <v>164</v>
+      </c>
+      <c r="G38" t="s">
+        <v>165</v>
+      </c>
+      <c r="H38" t="s">
+        <v>151</v>
+      </c>
+      <c r="K38" t="str">
+        <f>_xlfn.TEXTJOIN("", TRUE, D38:J38)</f>
+        <v>02_Slots/Gottheit/Goetter-mit-Epitheta/0001_Amun/epitheta/01_m-jp.t/0001_m-jp.t_01.png</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>216</v>
+      </c>
+      <c r="B39">
+        <v>1</v>
+      </c>
+      <c r="C39" t="s">
+        <v>31</v>
+      </c>
+      <c r="K39" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.2">
@@ -2292,7 +2293,7 @@
         <v>144</v>
       </c>
       <c r="K41" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.2">
@@ -2306,7 +2307,7 @@
         <v>144</v>
       </c>
       <c r="K43" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.2">
@@ -2320,7 +2321,7 @@
         <v>144</v>
       </c>
       <c r="K44" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.2">
@@ -2334,7 +2335,7 @@
         <v>144</v>
       </c>
       <c r="K45" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.2">
@@ -2348,7 +2349,7 @@
         <v>144</v>
       </c>
       <c r="K46" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.2">
@@ -2362,7 +2363,7 @@
         <v>144</v>
       </c>
       <c r="K47" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.2">
@@ -2376,7 +2377,7 @@
         <v>144</v>
       </c>
       <c r="K48" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.2">
@@ -2390,7 +2391,7 @@
         <v>144</v>
       </c>
       <c r="K49" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.2">
@@ -2404,7 +2405,7 @@
         <v>144</v>
       </c>
       <c r="K50" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.2">
@@ -2418,7 +2419,7 @@
         <v>144</v>
       </c>
       <c r="K51" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.2">
@@ -2432,7 +2433,7 @@
         <v>144</v>
       </c>
       <c r="K52" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.2">
@@ -2446,7 +2447,7 @@
         <v>144</v>
       </c>
       <c r="K53" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.2">
@@ -2460,7 +2461,7 @@
         <v>144</v>
       </c>
       <c r="K54" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.2">
@@ -2474,7 +2475,7 @@
         <v>144</v>
       </c>
       <c r="K55" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.2">
@@ -2488,7 +2489,7 @@
         <v>144</v>
       </c>
       <c r="K56" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.2">
@@ -2502,7 +2503,7 @@
         <v>144</v>
       </c>
       <c r="K57" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.2">
@@ -2516,7 +2517,7 @@
         <v>144</v>
       </c>
       <c r="K58" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.2">
@@ -2530,7 +2531,7 @@
         <v>144</v>
       </c>
       <c r="K59" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.2">
@@ -2544,7 +2545,7 @@
         <v>144</v>
       </c>
       <c r="K60" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.2">
@@ -2558,7 +2559,7 @@
         <v>144</v>
       </c>
       <c r="K61" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.2">
@@ -2572,7 +2573,7 @@
         <v>144</v>
       </c>
       <c r="K62" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.2">
@@ -2586,7 +2587,7 @@
         <v>144</v>
       </c>
       <c r="K63" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.2">
@@ -2600,7 +2601,7 @@
         <v>144</v>
       </c>
       <c r="K64" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.2">
@@ -2614,7 +2615,7 @@
         <v>144</v>
       </c>
       <c r="K65" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.2">
@@ -2628,7 +2629,7 @@
         <v>144</v>
       </c>
       <c r="K66" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.2">
@@ -2642,7 +2643,7 @@
         <v>144</v>
       </c>
       <c r="K67" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.2">
@@ -2656,7 +2657,7 @@
         <v>144</v>
       </c>
       <c r="K68" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.2">
@@ -2670,7 +2671,7 @@
         <v>144</v>
       </c>
       <c r="K69" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.2">
@@ -2684,7 +2685,7 @@
         <v>144</v>
       </c>
       <c r="K70" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.2">
@@ -2698,7 +2699,7 @@
         <v>144</v>
       </c>
       <c r="K71" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.2">
@@ -2712,7 +2713,7 @@
         <v>144</v>
       </c>
       <c r="K72" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.2">
@@ -2726,7 +2727,7 @@
         <v>144</v>
       </c>
       <c r="K73" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.2">
@@ -2740,7 +2741,7 @@
         <v>144</v>
       </c>
       <c r="K74" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.2">
@@ -2754,7 +2755,7 @@
         <v>144</v>
       </c>
       <c r="K75" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.2">
@@ -2768,7 +2769,7 @@
         <v>144</v>
       </c>
       <c r="K76" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.2">
@@ -2782,7 +2783,7 @@
         <v>144</v>
       </c>
       <c r="K77" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.2">
@@ -2796,7 +2797,7 @@
         <v>144</v>
       </c>
       <c r="K78" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.2">
@@ -2810,7 +2811,7 @@
         <v>144</v>
       </c>
       <c r="K79" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="80" spans="1:11" x14ac:dyDescent="0.2">
@@ -2824,7 +2825,7 @@
         <v>144</v>
       </c>
       <c r="K80" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.2">
@@ -2838,7 +2839,7 @@
         <v>144</v>
       </c>
       <c r="K81" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.2">
@@ -2852,7 +2853,7 @@
         <v>144</v>
       </c>
       <c r="K82" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.2">
@@ -2866,7 +2867,7 @@
         <v>144</v>
       </c>
       <c r="K83" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.2">
@@ -2880,7 +2881,7 @@
         <v>144</v>
       </c>
       <c r="K84" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
   </sheetData>
@@ -2893,7 +2894,7 @@
   <dimension ref="A1:G31"/>
   <sheetViews>
     <sheetView zoomScale="109" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B31"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.33203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>